<commit_message>
Tarea #2 Nataly Roa
Tarea #2 Analisis de datos
</commit_message>
<xml_diff>
--- a/Nataly Roa/Tarea_2.xlsx
+++ b/Nataly Roa/Tarea_2.xlsx
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">Scores</t>
   </si>
   <si>
     <t xml:space="preserve">1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nataly Roa</t>
   </si>
   <si>
     <t xml:space="preserve">Tablas de Frecuencias</t>
@@ -232,7 +235,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -269,23 +272,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -486,11 +477,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="96339960"/>
-        <c:axId val="76687128"/>
+        <c:axId val="99402095"/>
+        <c:axId val="98616950"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="96339960"/>
+        <c:axId val="99402095"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -556,7 +547,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76687128"/>
+        <c:crossAx val="98616950"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -564,7 +555,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76687128"/>
+        <c:axId val="98616950"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -637,7 +628,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96339960"/>
+        <c:crossAx val="99402095"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1152,9 +1143,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>702720</xdr:colOff>
+      <xdr:colOff>702360</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>130320</xdr:rowOff>
+      <xdr:rowOff>129960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1162,8 +1153,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7841160" y="3069360"/>
-        <a:ext cx="5839560" cy="2716560"/>
+        <a:off x="7844760" y="3069360"/>
+        <a:ext cx="5840640" cy="2716200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1182,9 +1173,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>813960</xdr:colOff>
+      <xdr:colOff>813600</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>120960</xdr:rowOff>
+      <xdr:rowOff>120600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1192,8 +1183,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="14020920" y="3060000"/>
-        <a:ext cx="5894280" cy="2716560"/>
+        <a:off x="14025960" y="3060000"/>
+        <a:ext cx="5893920" cy="2716200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1213,22 +1204,22 @@
   </sheetPr>
   <dimension ref="A1:N206"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="99" zoomScaleNormal="99" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="99" zoomScaleNormal="99" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8828125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.890625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="1" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.38"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="10.88"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="1" style="1" width="10.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.39"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="10.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="18.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="23.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="18.5"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="14" style="1" width="10.88"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="14" style="1" width="10.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1240,6 +1231,9 @@
       <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="n">
@@ -1263,7 +1257,7 @@
         <v>1277</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -1283,7 +1277,7 @@
         <v>1652</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F4" s="6" t="n">
         <f aca="false">MAX(A2:C31)</f>
@@ -1291,25 +1285,25 @@
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="N4" s="9" t="s">
         <v>10</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1323,7 +1317,7 @@
         <v>1592</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F5" s="6" t="n">
         <f aca="false">MIN(A2:C31)</f>
@@ -1369,7 +1363,7 @@
         <v>1477</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F6" s="6" t="n">
         <f aca="false">COUNT(A2:C31)</f>
@@ -1414,36 +1408,36 @@
         <v>1492</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F7" s="6" t="n">
         <f aca="false">F4-F5</f>
         <v>1197</v>
       </c>
       <c r="G7" s="7"/>
-      <c r="H7" s="10" t="n">
+      <c r="H7" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="I7" s="10" t="n">
+      <c r="I7" s="9" t="n">
         <f aca="false">J6+1</f>
         <v>1200</v>
       </c>
-      <c r="J7" s="10" t="n">
+      <c r="J7" s="9" t="n">
         <f aca="false">I7+200-1</f>
         <v>1399</v>
       </c>
-      <c r="K7" s="10" t="n">
+      <c r="K7" s="9" t="n">
         <v>18</v>
       </c>
-      <c r="L7" s="10" t="n">
+      <c r="L7" s="9" t="n">
         <f aca="false">L6+K7</f>
         <v>30</v>
       </c>
-      <c r="M7" s="10" t="n">
+      <c r="M7" s="9" t="n">
         <f aca="false">K7/90</f>
         <v>0.2</v>
       </c>
-      <c r="N7" s="10" t="n">
+      <c r="N7" s="9" t="n">
         <f aca="false">M7*100</f>
         <v>20</v>
       </c>
@@ -1459,36 +1453,36 @@
         <v>1527</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F8" s="6" t="n">
         <f aca="false">(F7)/200</f>
         <v>5.985</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="H8" s="11" t="n">
+      <c r="H8" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="I8" s="11" t="n">
+      <c r="I8" s="10" t="n">
         <f aca="false">J7+1</f>
         <v>1400</v>
       </c>
-      <c r="J8" s="11" t="n">
+      <c r="J8" s="10" t="n">
         <f aca="false">I8+200-1</f>
         <v>1599</v>
       </c>
-      <c r="K8" s="11" t="n">
+      <c r="K8" s="10" t="n">
         <v>30</v>
       </c>
-      <c r="L8" s="11" t="n">
+      <c r="L8" s="10" t="n">
         <f aca="false">L7+K8</f>
         <v>60</v>
       </c>
-      <c r="M8" s="11" t="n">
+      <c r="M8" s="10" t="n">
         <f aca="false">K8/90</f>
         <v>0.333333333333333</v>
       </c>
-      <c r="N8" s="11" t="n">
+      <c r="N8" s="10" t="n">
         <f aca="false">M8*100</f>
         <v>33.3333333333333</v>
       </c>
@@ -1504,7 +1498,7 @@
         <v>2137</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F9" s="6" t="n">
         <f aca="false">200</f>
@@ -1548,8 +1542,8 @@
       <c r="C10" s="1" t="n">
         <v>1562</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
       <c r="H10" s="6" t="n">
         <v>6</v>
       </c>
@@ -1669,11 +1663,11 @@
         <v>90</v>
       </c>
       <c r="L13" s="6"/>
-      <c r="M13" s="13" t="n">
+      <c r="M13" s="6" t="n">
         <f aca="false">SUM(M5:M12)</f>
         <v>1</v>
       </c>
-      <c r="N13" s="13" t="n">
+      <c r="N13" s="6" t="n">
         <f aca="false">M13*100</f>
         <v>100</v>
       </c>
@@ -1927,14 +1921,14 @@
         <v>1177</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H32" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I32" s="7"/>
       <c r="J32" s="7"/>
@@ -1946,14 +1940,14 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H34" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H35" s="12" t="s">
-        <v>19</v>
+      <c r="H35" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
@@ -1964,15 +1958,15 @@
       <c r="J36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H37" s="14" t="s">
-        <v>20</v>
+      <c r="H37" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H38" s="12" t="s">
-        <v>21</v>
+      <c r="H38" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
@@ -1983,18 +1977,18 @@
       <c r="J39" s="7"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H40" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="I40" s="15" t="n">
+      <c r="H40" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="I40" s="12" t="n">
         <f aca="false">AVERAGE(2400,2)</f>
         <v>1201</v>
       </c>
       <c r="J40" s="7"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H41" s="15"/>
-      <c r="I41" s="15"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
       <c r="J41" s="7"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2004,7 +1998,7 @@
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H43" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I43" s="7"/>
       <c r="J43" s="7"/>

</xml_diff>